<commit_message>
Update cement production restriction. Modify Uncertainty Table: AFOLU emission factor cells.
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/_GDP_Ref.xlsx
+++ b/t3a_experiments/Experiment_1/_GDP_Ref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\Dropbox\2_WORK\EperLab\2_Herramientas\_multipurpose_model_fmwk_v2\t3a_experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\Dropbox\2_WORK\EperLab\2_Herramientas\_mmf_GUA\OSeMOSYS_GUA_RDM_v20220213\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3921A4-E698-47E4-95C7-A1D383FCDE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAECB850-8779-4D04-BDEB-D9EE599BA306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25635" yWindow="2955" windowWidth="21510" windowHeight="10710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP" sheetId="1" r:id="rId1"/>
@@ -40,24 +40,6 @@
     <author>Luis Fernando Victor</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{57BBC434-1898-4A87-A230-DD62787302A0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">GDP in 2018 (real): 35,242,044.5 USD
-https://gee.bccr.fi.cr/indicadoreseconomicos/Cuadros/frmVerCatCuadro.aspx?idioma=1&amp;CodCuadro=%205784
-Exchange rate in 2018: 577 CRC/US$
-https://gee.bccr.fi.cr/indicadoreseconomicos/Cuadros/frmVerCatCuadro.aspx?idioma=1&amp;CodCuadro=%205790
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{0A973990-6DF2-4489-90EC-E92DA7AD7E35}">
       <text>
         <r>
@@ -601,19 +583,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="13.53515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.61328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -624,183 +609,174 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>2018</v>
       </c>
       <c r="B2" s="2">
-        <f>35242044.5/577</f>
-        <v>61078.066724436743</v>
+        <v>68004</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>2019</v>
       </c>
       <c r="B3" s="2">
-        <f>B2*(1+C3/100)</f>
-        <v>62482.86225909878</v>
-      </c>
-      <c r="C3">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+        <v>70634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2020</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B34" si="0">B3*(1+C4/100)</f>
-        <v>59921.064906475731</v>
-      </c>
-      <c r="C4">
-        <v>-4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+        <v>69561</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>2021</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
-        <v>62257.98643782828</v>
+        <f t="shared" ref="B5:B34" si="0">B4*(1+C5/100)</f>
+        <v>71995.634999999995</v>
       </c>
       <c r="C5">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>2022</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>64561.531936027925</v>
+        <v>74515.482224999985</v>
       </c>
       <c r="C6">
-        <v>3.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>2023</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>66498.377894108766</v>
+        <v>77123.524102874973</v>
       </c>
       <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>2024</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>68493.329230932024</v>
+        <v>79822.847446475585</v>
       </c>
       <c r="C8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>2025</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>70548.12910785999</v>
+        <v>82616.647107102224</v>
       </c>
       <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>2026</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>72664.572981095786</v>
+        <v>85508.2297558508</v>
       </c>
       <c r="C10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>2027</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>74844.510170528665</v>
+        <v>88501.017797305569</v>
       </c>
       <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>2028</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>77089.845475644528</v>
+        <v>91598.553420211261</v>
       </c>
       <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>2029</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>79402.540839913869</v>
+        <v>94804.502789918653</v>
       </c>
       <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>2030</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>81784.617065111292</v>
+        <v>98122.660387565804</v>
       </c>
       <c r="C14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>2031</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>84238.155577064637</v>
+        <v>101556.9535011306</v>
       </c>
       <c r="C15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>2032</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>86765.300244376573</v>
+        <v>105111.44687367017</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -809,10 +785,10 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>89368.259251707874</v>
+        <v>108790.34751424861</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
@@ -821,10 +797,10 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>92049.307029259115</v>
+        <v>112598.0096772473</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
@@ -833,10 +809,10 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>94810.786240136891</v>
+        <v>116538.94001595095</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
@@ -845,10 +821,10 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>97655.109827341003</v>
+        <v>120617.80291650923</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
@@ -857,10 +833,10 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>100584.76312216124</v>
+        <v>124839.42601858704</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
@@ -869,10 +845,10 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>103602.30601582608</v>
+        <v>129208.80592923757</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
@@ -881,10 +857,10 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>106710.37519630087</v>
+        <v>133731.11413676088</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
@@ -893,10 +869,10 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>109911.6864521899</v>
+        <v>138411.70313154749</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
@@ -905,10 +881,10 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>113209.0370457556</v>
+        <v>143256.11274115165</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
@@ -917,10 +893,10 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>116605.30815712827</v>
+        <v>148270.07668709193</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
@@ -929,10 +905,10 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>120103.46740184212</v>
+        <v>153459.52937114015</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
@@ -941,10 +917,10 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>123706.57142389739</v>
+        <v>158830.61289913004</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
@@ -953,10 +929,10 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>127417.76856661431</v>
+        <v>164389.68435059956</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
@@ -965,10 +941,10 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>131240.30162361273</v>
+        <v>170143.32330287053</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
@@ -977,10 +953,10 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" si="0"/>
-        <v>135177.51067232111</v>
+        <v>176098.33961847099</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
@@ -989,10 +965,10 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>139232.83599249076</v>
+        <v>182261.78150511745</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
@@ -1001,10 +977,10 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" si="0"/>
-        <v>143409.82107226548</v>
+        <v>188640.94385779655</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
@@ -1013,10 +989,10 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" si="0"/>
-        <v>147712.11570443344</v>
+        <v>195243.37689281942</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>
@@ -1030,7 +1006,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93394259-0791-4AF3-A5C0-DFDE9EDD707A}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1054,10 +1032,10 @@
         <v>2019</v>
       </c>
       <c r="B2" s="8">
-        <v>0.91600000000000004</v>
+        <v>2.4</v>
       </c>
       <c r="C2" s="8">
-        <v>1.0149999999999999</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1065,10 +1043,10 @@
         <v>2020</v>
       </c>
       <c r="B3" s="1">
-        <v>6</v>
+        <v>-6.2</v>
       </c>
       <c r="C3" s="1">
-        <v>1.0149999999999999</v>
+        <v>-3.6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1076,10 +1054,10 @@
         <v>2021</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>1.6</v>
       </c>
       <c r="C4" s="1">
-        <v>1.0149999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1087,10 +1065,10 @@
         <v>2022</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>1.6</v>
       </c>
       <c r="C5" s="1">
-        <v>1.0149999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1098,10 +1076,10 @@
         <v>2023</v>
       </c>
       <c r="B6" s="1">
-        <v>0.91600000000000004</v>
+        <v>1.6</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0149999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -1109,10 +1087,10 @@
         <v>2024</v>
       </c>
       <c r="B7" s="1">
-        <v>0.91600000000000004</v>
+        <v>1.6</v>
       </c>
       <c r="C7" s="1">
-        <v>1.0149999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -1298,7 +1276,7 @@
         <v>0.8</v>
       </c>
       <c r="C33" s="11">
-        <v>1.0149999999999999</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1310,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EF900E-2E45-49F0-9922-4F93E1E42E25}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1337,10 +1315,10 @@
         <v>2018</v>
       </c>
       <c r="B2" s="15">
-        <v>594.76997141865593</v>
+        <v>569.69220119404747</v>
       </c>
       <c r="C2" s="15">
-        <v>258.42337268486227</v>
+        <v>617.84772289277112</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1348,10 +1326,10 @@
         <v>2019</v>
       </c>
       <c r="B3" s="16">
-        <v>595.56330575398863</v>
+        <v>572.09535039782543</v>
       </c>
       <c r="C3" s="16">
-        <v>257.55382225078165</v>
+        <v>726.66152336268647</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1359,10 +1337,10 @@
         <v>2020</v>
       </c>
       <c r="B4" s="16">
-        <v>634.37791132934183</v>
+        <v>565.7144974914105</v>
       </c>
       <c r="C4" s="16">
-        <v>274.31922355945284</v>
+        <v>757.1376149652823</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1370,10 +1348,10 @@
         <v>2021</v>
       </c>
       <c r="B5" s="16">
-        <v>618.42989474850503</v>
+        <v>560.69234983613035</v>
       </c>
       <c r="C5" s="16">
-        <v>269.22007856354099</v>
+        <v>749.24155834931821</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -1381,10 +1359,10 @@
         <v>2022</v>
       </c>
       <c r="B6" s="16">
-        <v>603.94477687790311</v>
+        <v>560.69234983613035</v>
       </c>
       <c r="C6" s="16">
-        <v>264.62816924680186</v>
+        <v>749.24155834931821</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -1392,10 +1370,10 @@
         <v>2023</v>
       </c>
       <c r="B7" s="16">
-        <v>593.71673791606463</v>
+        <v>560.69234983613035</v>
       </c>
       <c r="C7" s="16">
-        <v>261.93420879734146</v>
+        <v>749.24155834931821</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -1403,10 +1381,10 @@
         <v>2024</v>
       </c>
       <c r="B8" s="16">
-        <v>583.56923876827739</v>
+        <v>560.69234983613035</v>
       </c>
       <c r="C8" s="16">
-        <v>259.06026468905736</v>
+        <v>749.24155834931821</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -1589,10 +1567,10 @@
         <v>2050</v>
       </c>
       <c r="B34" s="17">
-        <v>594.76997141865593</v>
+        <v>392.49492137322432</v>
       </c>
       <c r="C34" s="17">
-        <v>258.42337268486227</v>
+        <v>497.92920331860444</v>
       </c>
     </row>
   </sheetData>
@@ -1601,10 +1579,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BAD73B84EC2FBA4AB6031CFB79C3D0E0" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="371947e8e2760f0f8e8f59c32e4ad2a0">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4f98862-adfd-4d9c-a945-852f80f0eb51" xmlns:ns3="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a059f82d0b353b49693c069f8347eedf" ns2:_="" ns3:_="">
-    <xsd:import namespace="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
-    <xsd:import namespace="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
+    <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <xsd:import namespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -1613,15 +1591,17 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
@@ -1630,7 +1610,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c4f98862-adfd-4d9c-a945-852f80f0eb51" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -1643,55 +1623,67 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="13" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="17" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="20" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -1710,7 +1702,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -1727,8 +1719,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1827,9 +1819,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB2602C-E005-4B5F-A335-8D8F68706276}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DED5BB0D-7B00-45CF-80C4-8211BF791D8D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B1DA766-FA9C-4C8B-8AF4-A0AD061F6FEA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81950BC9-CD5C-4060-8364-5AFB53222010}"/>
 </file>
</xml_diff>